<commit_message>
[V&V] Alteração dos status dos RAN - Aprovada para resolução
Alteração nos status no Registro de Anomalias
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/6-Verificacao e Validacao/Registro de Anomalias.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/6-Verificacao e Validacao/Registro de Anomalias.xlsx
@@ -50,7 +50,7 @@
     <t>[AAQ-001]RA</t>
   </si>
   <si>
-    <t>Em avaliação</t>
+    <t>Aprovada para resolução</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +445,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="6">
-        <v>42158</v>
+        <v>42164</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -459,7 +459,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="6">
-        <v>42158</v>
+        <v>42164</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -473,7 +473,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="6">
-        <v>42158</v>
+        <v>42164</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -487,7 +487,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="6">
-        <v>42161</v>
+        <v>42164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[V&V] Alteração do status das anomalias - encerrado
As anomalias AAQ-001, AIM-001, AIM-002, AIM-003 foram reparadas e
encerradas
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/6-Verificacao e Validacao/Registro de Anomalias.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/6-Verificacao e Validacao/Registro de Anomalias.xlsx
@@ -50,7 +50,7 @@
     <t>[AAQ-001]RA</t>
   </si>
   <si>
-    <t>Aprovada para resolução</t>
+    <t>Reparada e encerrada.</t>
   </si>
 </sst>
 </file>
@@ -445,7 +445,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="6">
-        <v>42164</v>
+        <v>42165</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -459,7 +459,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="6">
-        <v>42164</v>
+        <v>42165</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -473,7 +473,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="6">
-        <v>42164</v>
+        <v>42165</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -487,7 +487,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="6">
-        <v>42164</v>
+        <v>42165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>